<commit_message>
Regenerate catalog content only to point to new data products
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="44">
   <si>
     <t>TileID</t>
   </si>
@@ -133,37 +133,13 @@
     <t>annually</t>
   </si>
   <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Delaware%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Fairfield%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Franklin%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Knox%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Licking%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Madison%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Marion%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Morrow%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Pickaway%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=Union%20County</t>
-  </si>
-  <si>
-    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831#geoName=10-County%20Region</t>
+    <t>https://www.arcgis.com/apps/dashboards/025b75f3490b4e79ae764e2c27c09a06</t>
+  </si>
+  <si>
+    <t>https://www.arcgis.com/apps/dashboards/d1bb7ef5468f495788703352b1c5f896</t>
+  </si>
+  <si>
+    <t>https://www.arcgis.com/apps/dashboards/2d3cc0a173d949f0a1a39146b37e1831</t>
   </si>
   <si>
     <t>https://morpc1-my.sharepoint.com/:w:/g/personal/aporr_morpc_org/EdF9OgInIZdOk9Sz3aJSVT8BPvXp4N495QUN2PvK5NBBjQ?e=b30KGA</t>
@@ -628,10 +604,10 @@
         <v>39</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -663,13 +639,13 @@
         <v>38</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -701,13 +677,13 @@
         <v>38</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -739,13 +715,13 @@
         <v>38</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -777,13 +753,13 @@
         <v>38</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -815,13 +791,13 @@
         <v>38</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -853,13 +829,13 @@
         <v>38</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -891,13 +867,13 @@
         <v>38</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -929,13 +905,13 @@
         <v>38</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -967,13 +943,13 @@
         <v>38</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1005,13 +981,13 @@
         <v>38</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1043,13 +1019,13 @@
         <v>38</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1084,10 +1060,10 @@
         <v>40</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1119,13 +1095,13 @@
         <v>38</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1157,13 +1133,13 @@
         <v>38</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -1195,13 +1171,13 @@
         <v>38</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -1233,13 +1209,13 @@
         <v>38</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="2:16">
@@ -1271,13 +1247,13 @@
         <v>38</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="2:16">
@@ -1309,13 +1285,13 @@
         <v>38</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="2:16">
@@ -1347,13 +1323,13 @@
         <v>38</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:16">
@@ -1385,13 +1361,13 @@
         <v>38</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="2:16">
@@ -1423,13 +1399,13 @@
         <v>38</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -1461,13 +1437,13 @@
         <v>38</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -1499,13 +1475,13 @@
         <v>38</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -1540,10 +1516,10 @@
         <v>41</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -1575,13 +1551,13 @@
         <v>38</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="2:16">
@@ -1613,13 +1589,13 @@
         <v>38</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:16">
@@ -1651,13 +1627,13 @@
         <v>38</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:16">
@@ -1689,13 +1665,13 @@
         <v>38</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="2:16">
@@ -1727,13 +1703,13 @@
         <v>38</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -1765,13 +1741,13 @@
         <v>38</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:16">
@@ -1803,13 +1779,13 @@
         <v>38</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="2:16">
@@ -1841,147 +1817,147 @@
         <v>38</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
-    <hyperlink ref="N2" r:id="rId2" location="geoName=Delaware%20County"/>
+    <hyperlink ref="N2" r:id="rId2"/>
     <hyperlink ref="O2" r:id="rId3"/>
     <hyperlink ref="P2" r:id="rId4"/>
     <hyperlink ref="I3" r:id="rId5"/>
-    <hyperlink ref="N3" r:id="rId6" location="geoName=Fairfield%20County"/>
+    <hyperlink ref="N3" r:id="rId6"/>
     <hyperlink ref="O3" r:id="rId7"/>
     <hyperlink ref="P3" r:id="rId8"/>
     <hyperlink ref="I4" r:id="rId9"/>
-    <hyperlink ref="N4" r:id="rId10" location="geoName=Franklin%20County"/>
+    <hyperlink ref="N4" r:id="rId10"/>
     <hyperlink ref="O4" r:id="rId11"/>
     <hyperlink ref="P4" r:id="rId12"/>
     <hyperlink ref="I5" r:id="rId13"/>
-    <hyperlink ref="N5" r:id="rId14" location="geoName=Knox%20County"/>
+    <hyperlink ref="N5" r:id="rId14"/>
     <hyperlink ref="O5" r:id="rId15"/>
     <hyperlink ref="P5" r:id="rId16"/>
     <hyperlink ref="I6" r:id="rId17"/>
-    <hyperlink ref="N6" r:id="rId18" location="geoName=Licking%20County"/>
+    <hyperlink ref="N6" r:id="rId18"/>
     <hyperlink ref="O6" r:id="rId19"/>
     <hyperlink ref="P6" r:id="rId20"/>
     <hyperlink ref="I7" r:id="rId21"/>
-    <hyperlink ref="N7" r:id="rId22" location="geoName=Madison%20County"/>
+    <hyperlink ref="N7" r:id="rId22"/>
     <hyperlink ref="O7" r:id="rId23"/>
     <hyperlink ref="P7" r:id="rId24"/>
     <hyperlink ref="I8" r:id="rId25"/>
-    <hyperlink ref="N8" r:id="rId26" location="geoName=Marion%20County"/>
+    <hyperlink ref="N8" r:id="rId26"/>
     <hyperlink ref="O8" r:id="rId27"/>
     <hyperlink ref="P8" r:id="rId28"/>
     <hyperlink ref="I9" r:id="rId29"/>
-    <hyperlink ref="N9" r:id="rId30" location="geoName=Morrow%20County"/>
+    <hyperlink ref="N9" r:id="rId30"/>
     <hyperlink ref="O9" r:id="rId31"/>
     <hyperlink ref="P9" r:id="rId32"/>
     <hyperlink ref="I10" r:id="rId33"/>
-    <hyperlink ref="N10" r:id="rId34" location="geoName=Pickaway%20County"/>
+    <hyperlink ref="N10" r:id="rId34"/>
     <hyperlink ref="O10" r:id="rId35"/>
     <hyperlink ref="P10" r:id="rId36"/>
     <hyperlink ref="I11" r:id="rId37"/>
-    <hyperlink ref="N11" r:id="rId38" location="geoName=Union%20County"/>
+    <hyperlink ref="N11" r:id="rId38"/>
     <hyperlink ref="O11" r:id="rId39"/>
     <hyperlink ref="P11" r:id="rId40"/>
     <hyperlink ref="I12" r:id="rId41"/>
-    <hyperlink ref="N12" r:id="rId42" location="geoName=10-County%20Region"/>
+    <hyperlink ref="N12" r:id="rId42"/>
     <hyperlink ref="O12" r:id="rId43"/>
     <hyperlink ref="P12" r:id="rId44"/>
     <hyperlink ref="I13" r:id="rId45"/>
-    <hyperlink ref="N13" r:id="rId46" location="geoName=Delaware%20County"/>
+    <hyperlink ref="N13" r:id="rId46"/>
     <hyperlink ref="O13" r:id="rId47"/>
     <hyperlink ref="P13" r:id="rId48"/>
     <hyperlink ref="I14" r:id="rId49"/>
-    <hyperlink ref="N14" r:id="rId50" location="geoName=Fairfield%20County"/>
+    <hyperlink ref="N14" r:id="rId50"/>
     <hyperlink ref="O14" r:id="rId51"/>
     <hyperlink ref="P14" r:id="rId52"/>
     <hyperlink ref="I15" r:id="rId53"/>
-    <hyperlink ref="N15" r:id="rId54" location="geoName=Franklin%20County"/>
+    <hyperlink ref="N15" r:id="rId54"/>
     <hyperlink ref="O15" r:id="rId55"/>
     <hyperlink ref="P15" r:id="rId56"/>
     <hyperlink ref="I16" r:id="rId57"/>
-    <hyperlink ref="N16" r:id="rId58" location="geoName=Knox%20County"/>
+    <hyperlink ref="N16" r:id="rId58"/>
     <hyperlink ref="O16" r:id="rId59"/>
     <hyperlink ref="P16" r:id="rId60"/>
     <hyperlink ref="I17" r:id="rId61"/>
-    <hyperlink ref="N17" r:id="rId62" location="geoName=Licking%20County"/>
+    <hyperlink ref="N17" r:id="rId62"/>
     <hyperlink ref="O17" r:id="rId63"/>
     <hyperlink ref="P17" r:id="rId64"/>
     <hyperlink ref="I18" r:id="rId65"/>
-    <hyperlink ref="N18" r:id="rId66" location="geoName=Madison%20County"/>
+    <hyperlink ref="N18" r:id="rId66"/>
     <hyperlink ref="O18" r:id="rId67"/>
     <hyperlink ref="P18" r:id="rId68"/>
     <hyperlink ref="I19" r:id="rId69"/>
-    <hyperlink ref="N19" r:id="rId70" location="geoName=Marion%20County"/>
+    <hyperlink ref="N19" r:id="rId70"/>
     <hyperlink ref="O19" r:id="rId71"/>
     <hyperlink ref="P19" r:id="rId72"/>
     <hyperlink ref="I20" r:id="rId73"/>
-    <hyperlink ref="N20" r:id="rId74" location="geoName=Morrow%20County"/>
+    <hyperlink ref="N20" r:id="rId74"/>
     <hyperlink ref="O20" r:id="rId75"/>
     <hyperlink ref="P20" r:id="rId76"/>
     <hyperlink ref="I21" r:id="rId77"/>
-    <hyperlink ref="N21" r:id="rId78" location="geoName=Pickaway%20County"/>
+    <hyperlink ref="N21" r:id="rId78"/>
     <hyperlink ref="O21" r:id="rId79"/>
     <hyperlink ref="P21" r:id="rId80"/>
     <hyperlink ref="I22" r:id="rId81"/>
-    <hyperlink ref="N22" r:id="rId82" location="geoName=Union%20County"/>
+    <hyperlink ref="N22" r:id="rId82"/>
     <hyperlink ref="O22" r:id="rId83"/>
     <hyperlink ref="P22" r:id="rId84"/>
     <hyperlink ref="I23" r:id="rId85"/>
-    <hyperlink ref="N23" r:id="rId86" location="geoName=10-County%20Region"/>
+    <hyperlink ref="N23" r:id="rId86"/>
     <hyperlink ref="O23" r:id="rId87"/>
     <hyperlink ref="P23" r:id="rId88"/>
     <hyperlink ref="I24" r:id="rId89"/>
-    <hyperlink ref="N24" r:id="rId90" location="geoName=Delaware%20County"/>
+    <hyperlink ref="N24" r:id="rId90"/>
     <hyperlink ref="O24" r:id="rId91"/>
     <hyperlink ref="P24" r:id="rId92"/>
     <hyperlink ref="I25" r:id="rId93"/>
-    <hyperlink ref="N25" r:id="rId94" location="geoName=Fairfield%20County"/>
+    <hyperlink ref="N25" r:id="rId94"/>
     <hyperlink ref="O25" r:id="rId95"/>
     <hyperlink ref="P25" r:id="rId96"/>
     <hyperlink ref="I26" r:id="rId97"/>
-    <hyperlink ref="N26" r:id="rId98" location="geoName=Franklin%20County"/>
+    <hyperlink ref="N26" r:id="rId98"/>
     <hyperlink ref="O26" r:id="rId99"/>
     <hyperlink ref="P26" r:id="rId100"/>
     <hyperlink ref="I27" r:id="rId101"/>
-    <hyperlink ref="N27" r:id="rId102" location="geoName=Knox%20County"/>
+    <hyperlink ref="N27" r:id="rId102"/>
     <hyperlink ref="O27" r:id="rId103"/>
     <hyperlink ref="P27" r:id="rId104"/>
     <hyperlink ref="I28" r:id="rId105"/>
-    <hyperlink ref="N28" r:id="rId106" location="geoName=Licking%20County"/>
+    <hyperlink ref="N28" r:id="rId106"/>
     <hyperlink ref="O28" r:id="rId107"/>
     <hyperlink ref="P28" r:id="rId108"/>
     <hyperlink ref="I29" r:id="rId109"/>
-    <hyperlink ref="N29" r:id="rId110" location="geoName=Madison%20County"/>
+    <hyperlink ref="N29" r:id="rId110"/>
     <hyperlink ref="O29" r:id="rId111"/>
     <hyperlink ref="P29" r:id="rId112"/>
     <hyperlink ref="I30" r:id="rId113"/>
-    <hyperlink ref="N30" r:id="rId114" location="geoName=Marion%20County"/>
+    <hyperlink ref="N30" r:id="rId114"/>
     <hyperlink ref="O30" r:id="rId115"/>
     <hyperlink ref="P30" r:id="rId116"/>
     <hyperlink ref="I31" r:id="rId117"/>
-    <hyperlink ref="N31" r:id="rId118" location="geoName=Morrow%20County"/>
+    <hyperlink ref="N31" r:id="rId118"/>
     <hyperlink ref="O31" r:id="rId119"/>
     <hyperlink ref="P31" r:id="rId120"/>
     <hyperlink ref="I32" r:id="rId121"/>
-    <hyperlink ref="N32" r:id="rId122" location="geoName=Pickaway%20County"/>
+    <hyperlink ref="N32" r:id="rId122"/>
     <hyperlink ref="O32" r:id="rId123"/>
     <hyperlink ref="P32" r:id="rId124"/>
     <hyperlink ref="I33" r:id="rId125"/>
-    <hyperlink ref="N33" r:id="rId126" location="geoName=Union%20County"/>
+    <hyperlink ref="N33" r:id="rId126"/>
     <hyperlink ref="O33" r:id="rId127"/>
     <hyperlink ref="P33" r:id="rId128"/>
     <hyperlink ref="I34" r:id="rId129"/>
-    <hyperlink ref="N34" r:id="rId130" location="geoName=10-County%20Region"/>
+    <hyperlink ref="N34" r:id="rId130"/>
     <hyperlink ref="O34" r:id="rId131"/>
     <hyperlink ref="P34" r:id="rId132"/>
   </hyperlinks>

</xml_diff>

<commit_message>
Correct generation of thumbnail URLs in catalog
</commit_message>
<xml_diff>
--- a/catalog.xlsx
+++ b/catalog.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="74">
   <si>
     <t>TileID</t>
   </si>
@@ -118,10 +118,100 @@
     <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Delaware.svg</t>
   </si>
   <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Fairfield.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Franklin.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Knox.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Licking.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Madison.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Marion.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Morrow.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Pickaway.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Union.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByType-Region10.svg</t>
+  </si>
+  <si>
     <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Delaware.svg</t>
   </si>
   <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Fairfield.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Franklin.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Knox.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Licking.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Madison.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Marion.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Morrow.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Pickaway.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Union.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByYear-Region10.svg</t>
+  </si>
+  <si>
     <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Delaware.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Fairfield.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Franklin.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Knox.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Licking.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Madison.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Marion.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Morrow.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Pickaway.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Union.svg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/morpc-insights/insights-crashes/refs/heads/main/output_data/charts/crashSeverityByMode-Region10.svg</t>
   </si>
   <si>
     <t>Mid-Ohio Regional Planning Commission</t>
@@ -592,22 +682,22 @@
         <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -627,25 +717,25 @@
         <v>32</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L3" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -665,25 +755,25 @@
         <v>32</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K4" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -703,25 +793,25 @@
         <v>32</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K5" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L5" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -741,25 +831,25 @@
         <v>32</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L6" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -779,25 +869,25 @@
         <v>32</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K7" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L7" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -817,25 +907,25 @@
         <v>32</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K8" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L8" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -855,25 +945,25 @@
         <v>32</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K9" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L9" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -893,25 +983,25 @@
         <v>32</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="J10" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K10" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L10" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -931,25 +1021,25 @@
         <v>32</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K11" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L11" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -969,25 +1059,25 @@
         <v>32</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="J12" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K12" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L12" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1007,25 +1097,25 @@
         <v>32</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L13" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1045,25 +1135,25 @@
         <v>32</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="J14" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K14" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L14" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1083,25 +1173,25 @@
         <v>32</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="J15" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K15" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L15" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1121,25 +1211,25 @@
         <v>32</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="J16" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K16" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L16" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="2:16">
@@ -1159,25 +1249,25 @@
         <v>32</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="J17" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K17" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L17" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="18" spans="2:16">
@@ -1197,25 +1287,25 @@
         <v>32</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="J18" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K18" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L18" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="2:16">
@@ -1235,25 +1325,25 @@
         <v>32</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K19" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L19" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="2:16">
@@ -1273,25 +1363,25 @@
         <v>32</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="J20" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L20" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="2:16">
@@ -1311,25 +1401,25 @@
         <v>32</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="J21" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K21" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L21" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="2:16">
@@ -1349,25 +1439,25 @@
         <v>32</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="J22" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K22" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L22" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="2:16">
@@ -1387,25 +1477,25 @@
         <v>32</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="J23" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K23" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L23" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -1425,25 +1515,25 @@
         <v>32</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="J24" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K24" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L24" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -1463,25 +1553,25 @@
         <v>32</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="J25" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K25" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L25" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -1501,25 +1591,25 @@
         <v>32</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="J26" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K26" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L26" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="27" spans="2:16">
@@ -1539,25 +1629,25 @@
         <v>32</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="J27" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K27" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L27" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" spans="2:16">
@@ -1577,25 +1667,25 @@
         <v>32</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="J28" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K28" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L28" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="2:16">
@@ -1615,25 +1705,25 @@
         <v>32</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>35</v>
+        <v>60</v>
       </c>
       <c r="J29" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K29" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L29" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="2:16">
@@ -1653,25 +1743,25 @@
         <v>32</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="J30" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K30" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L30" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="2:16">
@@ -1691,25 +1781,25 @@
         <v>32</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="J31" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K31" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L31" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="2:16">
@@ -1729,25 +1819,25 @@
         <v>32</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="J32" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K32" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L32" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="2:16">
@@ -1767,25 +1857,25 @@
         <v>32</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="J33" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K33" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L33" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="2:16">
@@ -1805,25 +1895,25 @@
         <v>32</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="J34" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="K34" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="L34" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>